<commit_message>
Testing for bridge weights and comparing MCTS and Minimax
</commit_message>
<xml_diff>
--- a/parameterTuning/Results calculations/CandBTuning Results.xlsx
+++ b/parameterTuning/Results calculations/CandBTuning Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bae6c403b3f18583/Documents/Code/C^M^M/Projects/Hex/Hex-AI-Project/parameterTuning/Results calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{937EB215-A717-4548-90C0-6A6A995DA22A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="36" documentId="8_{937EB215-A717-4548-90C0-6A6A995DA22A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9602686C-B34D-4137-8A0B-5C238636E6C3}"/>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="1575" windowWidth="19230" windowHeight="11940" xr2:uid="{B55DC118-92EE-4A08-A67A-325C9A362869}"/>
+    <workbookView minimized="1" xWindow="9030" yWindow="2280" windowWidth="19230" windowHeight="11940" xr2:uid="{B55DC118-92EE-4A08-A67A-325C9A362869}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="8">
   <si>
     <t>Player 1 wins</t>
   </si>
@@ -51,6 +51,15 @@
   </si>
   <si>
     <t>b value</t>
+  </si>
+  <si>
+    <t>bridgeWeight</t>
+  </si>
+  <si>
+    <t>60Sec</t>
+  </si>
+  <si>
+    <t>10Sec</t>
   </si>
 </sst>
 </file>
@@ -403,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34E14E40-EAF8-4F55-8EA8-99746A3EAB76}">
-  <dimension ref="B4:J11"/>
+  <dimension ref="B3:T13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="U21" sqref="U21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -415,7 +424,15 @@
     <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="L3" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -440,8 +457,32 @@
       <c r="J4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="L4" t="s">
+        <v>5</v>
+      </c>
+      <c r="M4" t="s">
+        <v>0</v>
+      </c>
+      <c r="N4" t="s">
+        <v>1</v>
+      </c>
+      <c r="O4" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>5</v>
+      </c>
+      <c r="R4" t="s">
+        <v>0</v>
+      </c>
+      <c r="S4" t="s">
+        <v>1</v>
+      </c>
+      <c r="T4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>0</v>
       </c>
@@ -459,16 +500,47 @@
       <c r="G5">
         <v>5.0000000000000001E-4</v>
       </c>
+      <c r="H5">
+        <v>16</v>
+      </c>
       <c r="I5">
         <f>30-H5</f>
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="J5" s="1">
         <f>H5/30</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+        <v>0.53333333333333333</v>
+      </c>
+      <c r="L5">
+        <v>2.1</v>
+      </c>
+      <c r="M5">
+        <v>16</v>
+      </c>
+      <c r="N5">
+        <f>30-M5</f>
+        <v>14</v>
+      </c>
+      <c r="O5" s="1">
+        <f>M5/30</f>
+        <v>0.53333333333333333</v>
+      </c>
+      <c r="Q5">
+        <v>2.1</v>
+      </c>
+      <c r="R5">
+        <v>17</v>
+      </c>
+      <c r="S5">
+        <f>30-R5</f>
+        <v>13</v>
+      </c>
+      <c r="T5" s="1">
+        <f>R5/30</f>
+        <v>0.56666666666666665</v>
+      </c>
+    </row>
+    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>0.1</v>
       </c>
@@ -486,16 +558,47 @@
       <c r="G6">
         <v>2.5000000000000001E-4</v>
       </c>
+      <c r="H6">
+        <v>13</v>
+      </c>
       <c r="I6">
-        <f t="shared" ref="I6:I11" si="2">30-H6</f>
-        <v>30</v>
+        <f t="shared" ref="I6:I7" si="2">30-H6</f>
+        <v>17</v>
       </c>
       <c r="J6" s="1">
-        <f t="shared" ref="J6:J11" si="3">H6/30</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+        <f t="shared" ref="J6:J7" si="3">H6/30</f>
+        <v>0.43333333333333335</v>
+      </c>
+      <c r="L6">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="M6">
+        <v>16</v>
+      </c>
+      <c r="N6">
+        <f t="shared" ref="N6:N13" si="4">30-M6</f>
+        <v>14</v>
+      </c>
+      <c r="O6" s="1">
+        <f t="shared" ref="O6:O13" si="5">M6/30</f>
+        <v>0.53333333333333333</v>
+      </c>
+      <c r="Q6">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="R6">
+        <v>13</v>
+      </c>
+      <c r="S6">
+        <f t="shared" ref="S6:S13" si="6">30-R6</f>
+        <v>17</v>
+      </c>
+      <c r="T6" s="1">
+        <f t="shared" ref="T6:T13" si="7">R6/30</f>
+        <v>0.43333333333333335</v>
+      </c>
+    </row>
+    <row r="7" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>0.2</v>
       </c>
@@ -513,16 +616,47 @@
       <c r="G7">
         <v>1.25E-4</v>
       </c>
+      <c r="H7">
+        <v>14</v>
+      </c>
       <c r="I7">
         <f t="shared" si="2"/>
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="J7" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+        <v>0.46666666666666667</v>
+      </c>
+      <c r="L7">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="M7">
+        <v>20</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="O7" s="1">
+        <f t="shared" si="5"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="Q7">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="R7">
+        <v>11</v>
+      </c>
+      <c r="S7">
+        <f t="shared" si="6"/>
+        <v>19</v>
+      </c>
+      <c r="T7" s="1">
+        <f t="shared" si="7"/>
+        <v>0.36666666666666664</v>
+      </c>
+    </row>
+    <row r="8" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>0.4</v>
       </c>
@@ -538,8 +672,36 @@
         <v>0.5</v>
       </c>
       <c r="J8" s="1"/>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="L8">
+        <v>2.4</v>
+      </c>
+      <c r="M8">
+        <v>15</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="4"/>
+        <v>15</v>
+      </c>
+      <c r="O8" s="1">
+        <f t="shared" si="5"/>
+        <v>0.5</v>
+      </c>
+      <c r="Q8">
+        <v>2.4</v>
+      </c>
+      <c r="R8">
+        <v>16</v>
+      </c>
+      <c r="S8">
+        <f t="shared" si="6"/>
+        <v>14</v>
+      </c>
+      <c r="T8" s="1">
+        <f t="shared" si="7"/>
+        <v>0.53333333333333333</v>
+      </c>
+    </row>
+    <row r="9" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>0.5</v>
       </c>
@@ -555,8 +717,36 @@
         <v>0.46666666666666667</v>
       </c>
       <c r="J9" s="1"/>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="L9">
+        <v>2.5</v>
+      </c>
+      <c r="M9">
+        <v>16</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="4"/>
+        <v>14</v>
+      </c>
+      <c r="O9" s="1">
+        <f t="shared" si="5"/>
+        <v>0.53333333333333333</v>
+      </c>
+      <c r="Q9">
+        <v>2.5</v>
+      </c>
+      <c r="R9">
+        <v>14</v>
+      </c>
+      <c r="S9">
+        <f t="shared" si="6"/>
+        <v>16</v>
+      </c>
+      <c r="T9" s="1">
+        <f t="shared" si="7"/>
+        <v>0.46666666666666667</v>
+      </c>
+    </row>
+    <row r="10" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>0.6</v>
       </c>
@@ -572,8 +762,36 @@
         <v>0.4</v>
       </c>
       <c r="J10" s="1"/>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="L10">
+        <v>2.6</v>
+      </c>
+      <c r="M10">
+        <v>20</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="O10" s="1">
+        <f t="shared" si="5"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="Q10">
+        <v>2.6</v>
+      </c>
+      <c r="R10">
+        <v>13</v>
+      </c>
+      <c r="S10">
+        <f t="shared" si="6"/>
+        <v>17</v>
+      </c>
+      <c r="T10" s="1">
+        <f t="shared" si="7"/>
+        <v>0.43333333333333335</v>
+      </c>
+    </row>
+    <row r="11" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>0.7</v>
       </c>
@@ -589,6 +807,94 @@
         <v>0.43333333333333335</v>
       </c>
       <c r="J11" s="1"/>
+      <c r="L11">
+        <v>2.7</v>
+      </c>
+      <c r="M11">
+        <v>16</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="4"/>
+        <v>14</v>
+      </c>
+      <c r="O11" s="1">
+        <f t="shared" si="5"/>
+        <v>0.53333333333333333</v>
+      </c>
+      <c r="Q11">
+        <v>2.7</v>
+      </c>
+      <c r="R11">
+        <v>14</v>
+      </c>
+      <c r="S11">
+        <f t="shared" si="6"/>
+        <v>16</v>
+      </c>
+      <c r="T11" s="1">
+        <f t="shared" si="7"/>
+        <v>0.46666666666666667</v>
+      </c>
+    </row>
+    <row r="12" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="L12">
+        <v>2.8</v>
+      </c>
+      <c r="M12">
+        <v>14</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+      <c r="O12" s="1">
+        <f t="shared" si="5"/>
+        <v>0.46666666666666667</v>
+      </c>
+      <c r="Q12">
+        <v>2.8</v>
+      </c>
+      <c r="R12">
+        <v>15</v>
+      </c>
+      <c r="S12">
+        <f t="shared" si="6"/>
+        <v>15</v>
+      </c>
+      <c r="T12" s="1">
+        <f t="shared" si="7"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="13" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="L13">
+        <v>2.9</v>
+      </c>
+      <c r="M13">
+        <v>10</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="4"/>
+        <v>20</v>
+      </c>
+      <c r="O13" s="1">
+        <f t="shared" si="5"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="Q13">
+        <v>2.9</v>
+      </c>
+      <c r="R13">
+        <v>20</v>
+      </c>
+      <c r="S13">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="T13" s="1">
+        <f t="shared" si="7"/>
+        <v>0.66666666666666663</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>